<commit_message>
fix: game report template courts
</commit_message>
<xml_diff>
--- a/core/report/GBO_V2.xlsx
+++ b/core/report/GBO_V2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\makunz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\beach\to\core\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8910" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DBT" sheetId="1" r:id="rId1"/>
@@ -1639,168 +1639,18 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
@@ -1811,18 +1661,168 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="66" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="67" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="72" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2254,27 +2254,27 @@
   </sheetPr>
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="95" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="Y21" sqref="Y21"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" style="71" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" style="71" customWidth="1"/>
-    <col min="4" max="8" width="3.6640625" style="71" customWidth="1"/>
-    <col min="9" max="9" width="3.109375" style="71" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" style="71" customWidth="1"/>
-    <col min="11" max="11" width="3.6640625" style="71" customWidth="1"/>
-    <col min="12" max="12" width="3.88671875" style="71" customWidth="1"/>
-    <col min="13" max="15" width="3.6640625" style="71" customWidth="1"/>
-    <col min="16" max="16" width="3.44140625" style="71" customWidth="1"/>
-    <col min="17" max="22" width="3.6640625" style="71" customWidth="1"/>
-    <col min="23" max="23" width="4.33203125" style="71" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="71" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" style="71" customWidth="1"/>
+    <col min="4" max="8" width="3.7109375" style="71" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" style="71" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="71" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" style="71" customWidth="1"/>
+    <col min="12" max="12" width="3.85546875" style="71" customWidth="1"/>
+    <col min="13" max="15" width="3.7109375" style="71" customWidth="1"/>
+    <col min="16" max="16" width="3.42578125" style="71" customWidth="1"/>
+    <col min="17" max="22" width="3.7109375" style="71" customWidth="1"/>
+    <col min="23" max="23" width="4.28515625" style="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="36"/>
       <c r="B1" s="37" t="s">
         <v>0</v>
@@ -2301,7 +2301,7 @@
       <c r="V1" s="74"/>
       <c r="W1" s="74"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="36"/>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -2326,14 +2326,14 @@
       <c r="V2" s="38"/>
       <c r="W2" s="74"/>
     </row>
-    <row r="3" spans="1:23" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="36"/>
-      <c r="B3" s="177" t="s">
+      <c r="B3" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="161"/>
+      <c r="C3" s="170"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="177"/>
       <c r="F3" s="124"/>
       <c r="G3" s="39" t="s">
         <v>2</v>
@@ -2363,12 +2363,12 @@
       <c r="V3" s="39"/>
       <c r="W3" s="74"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="36"/>
-      <c r="B4" s="160"/>
-      <c r="C4" s="160"/>
-      <c r="D4" s="160"/>
-      <c r="E4" s="161"/>
+      <c r="B4" s="170"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="177"/>
       <c r="F4" s="124"/>
       <c r="G4" s="39" t="s">
         <v>8</v>
@@ -2396,12 +2396,12 @@
       <c r="V4" s="128"/>
       <c r="W4" s="74"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="36"/>
-      <c r="B5" s="160"/>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="161"/>
+      <c r="B5" s="170"/>
+      <c r="C5" s="170"/>
+      <c r="D5" s="170"/>
+      <c r="E5" s="177"/>
       <c r="F5" s="124"/>
       <c r="G5" s="39" t="s">
         <v>12</v>
@@ -2429,7 +2429,7 @@
       <c r="V5" s="131"/>
       <c r="W5" s="74"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="36"/>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
@@ -2454,27 +2454,27 @@
       <c r="V6" s="39"/>
       <c r="W6" s="74"/>
     </row>
-    <row r="7" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="36"/>
-      <c r="B7" s="141" t="s">
+      <c r="B7" s="190" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="142"/>
-      <c r="D7" s="142"/>
-      <c r="E7" s="142"/>
-      <c r="F7" s="143"/>
-      <c r="G7" s="144" t="s">
+      <c r="C7" s="179"/>
+      <c r="D7" s="179"/>
+      <c r="E7" s="179"/>
+      <c r="F7" s="180"/>
+      <c r="G7" s="191" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="142"/>
-      <c r="I7" s="142"/>
-      <c r="J7" s="142"/>
-      <c r="K7" s="142"/>
-      <c r="L7" s="142"/>
-      <c r="M7" s="142"/>
-      <c r="N7" s="142"/>
-      <c r="O7" s="142"/>
-      <c r="P7" s="143"/>
+      <c r="H7" s="179"/>
+      <c r="I7" s="179"/>
+      <c r="J7" s="179"/>
+      <c r="K7" s="179"/>
+      <c r="L7" s="179"/>
+      <c r="M7" s="179"/>
+      <c r="N7" s="179"/>
+      <c r="O7" s="179"/>
+      <c r="P7" s="180"/>
       <c r="Q7" s="40"/>
       <c r="R7" s="40" t="s">
         <v>17</v>
@@ -2487,89 +2487,85 @@
       <c r="V7" s="40"/>
       <c r="W7" s="74"/>
     </row>
-    <row r="8" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="36"/>
       <c r="B8" s="178"/>
-      <c r="C8" s="142"/>
-      <c r="D8" s="142"/>
-      <c r="E8" s="142"/>
-      <c r="F8" s="143"/>
+      <c r="C8" s="179"/>
+      <c r="D8" s="179"/>
+      <c r="E8" s="179"/>
+      <c r="F8" s="180"/>
       <c r="G8" s="178"/>
-      <c r="H8" s="142"/>
-      <c r="I8" s="142"/>
-      <c r="J8" s="142"/>
-      <c r="K8" s="142"/>
-      <c r="L8" s="142"/>
-      <c r="M8" s="142"/>
-      <c r="N8" s="142"/>
-      <c r="O8" s="142"/>
-      <c r="P8" s="143"/>
-      <c r="Q8" s="40">
-        <v>1</v>
-      </c>
+      <c r="H8" s="179"/>
+      <c r="I8" s="179"/>
+      <c r="J8" s="179"/>
+      <c r="K8" s="179"/>
+      <c r="L8" s="179"/>
+      <c r="M8" s="179"/>
+      <c r="N8" s="179"/>
+      <c r="O8" s="179"/>
+      <c r="P8" s="180"/>
+      <c r="Q8" s="40"/>
       <c r="R8" s="125"/>
       <c r="S8" s="40"/>
-      <c r="T8" s="171" t="str">
+      <c r="T8" s="183" t="str">
         <f>IF(M40="","",SUM(M42,T42,T46))</f>
         <v/>
       </c>
-      <c r="U8" s="174" t="s">
+      <c r="U8" s="185" t="s">
         <v>19</v>
       </c>
-      <c r="V8" s="175" t="str">
+      <c r="V8" s="186" t="str">
         <f>IF(O40="","",SUM(O42,V42,V46))</f>
         <v/>
       </c>
       <c r="W8" s="74"/>
     </row>
-    <row r="9" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36"/>
       <c r="B9" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="176" t="s">
+      <c r="C9" s="181" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="160"/>
-      <c r="E9" s="160"/>
-      <c r="F9" s="176" t="s">
+      <c r="D9" s="170"/>
+      <c r="E9" s="170"/>
+      <c r="F9" s="181" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="160"/>
-      <c r="H9" s="160"/>
-      <c r="I9" s="176" t="s">
+      <c r="G9" s="170"/>
+      <c r="H9" s="170"/>
+      <c r="I9" s="181" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="160"/>
-      <c r="K9" s="160"/>
-      <c r="L9" s="176" t="s">
+      <c r="J9" s="170"/>
+      <c r="K9" s="170"/>
+      <c r="L9" s="181" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="160"/>
-      <c r="N9" s="154" t="s">
+      <c r="M9" s="170"/>
+      <c r="N9" s="201" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="142"/>
-      <c r="P9" s="142"/>
-      <c r="Q9" s="40">
-        <v>2</v>
-      </c>
-      <c r="R9" s="125"/>
+      <c r="O9" s="179"/>
+      <c r="P9" s="179"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="74"/>
       <c r="S9" s="40"/>
-      <c r="T9" s="172"/>
-      <c r="U9" s="160"/>
-      <c r="V9" s="161"/>
+      <c r="T9" s="184"/>
+      <c r="U9" s="170"/>
+      <c r="V9" s="177"/>
       <c r="W9" s="74"/>
     </row>
-    <row r="10" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="36"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="142"/>
-      <c r="E10" s="143"/>
-      <c r="F10" s="170"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="143"/>
+      <c r="C10" s="182"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="180"/>
+      <c r="F10" s="182"/>
+      <c r="G10" s="179"/>
+      <c r="H10" s="180"/>
       <c r="I10" s="65"/>
       <c r="J10" s="66"/>
       <c r="K10" s="67"/>
@@ -2578,17 +2574,15 @@
       <c r="N10" s="65"/>
       <c r="O10" s="66"/>
       <c r="P10" s="68"/>
-      <c r="Q10" s="40">
-        <v>3</v>
-      </c>
-      <c r="R10" s="125"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="74"/>
       <c r="S10" s="40"/>
-      <c r="T10" s="173"/>
-      <c r="U10" s="163"/>
-      <c r="V10" s="164"/>
+      <c r="T10" s="150"/>
+      <c r="U10" s="135"/>
+      <c r="V10" s="151"/>
       <c r="W10" s="74"/>
     </row>
-    <row r="11" spans="1:23" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="75"/>
       <c r="B11" s="75"/>
       <c r="C11" s="75"/>
@@ -2613,7 +2607,7 @@
       <c r="V11" s="74"/>
       <c r="W11" s="74"/>
     </row>
-    <row r="12" spans="1:23" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>26</v>
       </c>
@@ -2637,26 +2631,26 @@
         <v>31</v>
       </c>
       <c r="I12" s="74"/>
-      <c r="J12" s="165" t="s">
+      <c r="J12" s="206" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="137"/>
-      <c r="L12" s="137"/>
-      <c r="M12" s="137"/>
-      <c r="N12" s="137"/>
-      <c r="O12" s="166"/>
+      <c r="K12" s="160"/>
+      <c r="L12" s="160"/>
+      <c r="M12" s="160"/>
+      <c r="N12" s="160"/>
+      <c r="O12" s="161"/>
       <c r="P12" s="74"/>
-      <c r="Q12" s="179" t="s">
+      <c r="Q12" s="159" t="s">
         <v>33</v>
       </c>
-      <c r="R12" s="137"/>
-      <c r="S12" s="137"/>
-      <c r="T12" s="137"/>
-      <c r="U12" s="137"/>
-      <c r="V12" s="166"/>
+      <c r="R12" s="160"/>
+      <c r="S12" s="160"/>
+      <c r="T12" s="160"/>
+      <c r="U12" s="160"/>
+      <c r="V12" s="161"/>
       <c r="W12" s="74"/>
     </row>
-    <row r="13" spans="1:23" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="22"/>
       <c r="C13" s="23"/>
@@ -2708,7 +2702,7 @@
       </c>
       <c r="W13" s="74"/>
     </row>
-    <row r="14" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="24"/>
       <c r="C14" s="23"/>
@@ -2744,7 +2738,7 @@
       <c r="V14" s="90"/>
       <c r="W14" s="74"/>
     </row>
-    <row r="15" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="24"/>
       <c r="C15" s="23"/>
@@ -2780,7 +2774,7 @@
       <c r="V15" s="91"/>
       <c r="W15" s="74"/>
     </row>
-    <row r="16" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="24"/>
       <c r="C16" s="23"/>
@@ -2816,7 +2810,7 @@
       <c r="V16" s="90"/>
       <c r="W16" s="74"/>
     </row>
-    <row r="17" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20"/>
       <c r="B17" s="24"/>
       <c r="C17" s="23"/>
@@ -2852,7 +2846,7 @@
       <c r="V17" s="91"/>
       <c r="W17" s="74"/>
     </row>
-    <row r="18" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="24"/>
       <c r="C18" s="23"/>
@@ -2888,7 +2882,7 @@
       <c r="V18" s="90"/>
       <c r="W18" s="74"/>
     </row>
-    <row r="19" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="24"/>
       <c r="C19" s="23"/>
@@ -2924,7 +2918,7 @@
       <c r="V19" s="91"/>
       <c r="W19" s="74"/>
     </row>
-    <row r="20" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="24"/>
       <c r="C20" s="23"/>
@@ -2960,7 +2954,7 @@
       <c r="V20" s="92"/>
       <c r="W20" s="74"/>
     </row>
-    <row r="21" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="24"/>
       <c r="C21" s="23"/>
@@ -2996,7 +2990,7 @@
       <c r="V21" s="91"/>
       <c r="W21" s="74"/>
     </row>
-    <row r="22" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="24"/>
       <c r="C22" s="23"/>
@@ -3032,7 +3026,7 @@
       <c r="V22" s="90"/>
       <c r="W22" s="74"/>
     </row>
-    <row r="23" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20"/>
       <c r="B23" s="24"/>
       <c r="C23" s="23"/>
@@ -3068,7 +3062,7 @@
       <c r="V23" s="91"/>
       <c r="W23" s="74"/>
     </row>
-    <row r="24" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="21"/>
       <c r="B24" s="25"/>
       <c r="C24" s="26"/>
@@ -3104,7 +3098,7 @@
       <c r="V24" s="90"/>
       <c r="W24" s="74"/>
     </row>
-    <row r="25" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="112" t="s">
         <v>34</v>
       </c>
@@ -3156,17 +3150,17 @@
       <c r="V25" s="91"/>
       <c r="W25" s="74"/>
     </row>
-    <row r="26" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="119" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="120"/>
       <c r="C26" s="117"/>
-      <c r="D26" s="145" t="s">
+      <c r="D26" s="192" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="146"/>
-      <c r="F26" s="147"/>
+      <c r="E26" s="193"/>
+      <c r="F26" s="194"/>
       <c r="G26" s="118" t="s">
         <v>38</v>
       </c>
@@ -3197,15 +3191,15 @@
       <c r="V26" s="90"/>
       <c r="W26" s="74"/>
     </row>
-    <row r="27" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="167" t="s">
+    <row r="27" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="207" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="133"/>
-      <c r="C27" s="133"/>
-      <c r="D27" s="148"/>
-      <c r="E27" s="149"/>
-      <c r="F27" s="150"/>
+      <c r="B27" s="146"/>
+      <c r="C27" s="146"/>
+      <c r="D27" s="195"/>
+      <c r="E27" s="196"/>
+      <c r="F27" s="197"/>
       <c r="G27" s="94"/>
       <c r="H27" s="94"/>
       <c r="I27" s="74"/>
@@ -3232,15 +3226,15 @@
       <c r="V27" s="91"/>
       <c r="W27" s="74"/>
     </row>
-    <row r="28" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="155"/>
-      <c r="B28" s="142"/>
-      <c r="C28" s="142"/>
-      <c r="D28" s="142"/>
-      <c r="E28" s="142"/>
-      <c r="F28" s="142"/>
-      <c r="G28" s="142"/>
-      <c r="H28" s="142"/>
+    <row r="28" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="202"/>
+      <c r="B28" s="179"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="179"/>
+      <c r="E28" s="179"/>
+      <c r="F28" s="179"/>
+      <c r="G28" s="179"/>
+      <c r="H28" s="179"/>
       <c r="I28" s="74"/>
       <c r="J28" s="78"/>
       <c r="K28" s="14">
@@ -3265,7 +3259,7 @@
       <c r="V28" s="90"/>
       <c r="W28" s="74"/>
     </row>
-    <row r="29" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>26</v>
       </c>
@@ -3312,7 +3306,7 @@
       <c r="V29" s="91"/>
       <c r="W29" s="74"/>
     </row>
-    <row r="30" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
       <c r="B30" s="24"/>
       <c r="C30" s="23"/>
@@ -3348,7 +3342,7 @@
       <c r="V30" s="92"/>
       <c r="W30" s="74"/>
     </row>
-    <row r="31" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20"/>
       <c r="B31" s="24"/>
       <c r="C31" s="23"/>
@@ -3384,7 +3378,7 @@
       <c r="V31" s="92"/>
       <c r="W31" s="74"/>
     </row>
-    <row r="32" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20"/>
       <c r="B32" s="24"/>
       <c r="C32" s="23"/>
@@ -3421,7 +3415,7 @@
       <c r="W32" s="74"/>
       <c r="X32" s="17"/>
     </row>
-    <row r="33" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
       <c r="B33" s="24"/>
       <c r="C33" s="23"/>
@@ -3457,7 +3451,7 @@
       <c r="V33" s="93"/>
       <c r="W33" s="74"/>
     </row>
-    <row r="34" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20"/>
       <c r="B34" s="24"/>
       <c r="C34" s="23"/>
@@ -3470,24 +3464,24 @@
       <c r="G34" s="94"/>
       <c r="H34" s="94"/>
       <c r="I34" s="74"/>
-      <c r="J34" s="190" t="s">
+      <c r="J34" s="169" t="s">
         <v>42</v>
       </c>
-      <c r="K34" s="160"/>
-      <c r="L34" s="160"/>
-      <c r="M34" s="160"/>
-      <c r="N34" s="160"/>
-      <c r="O34" s="160"/>
-      <c r="P34" s="160"/>
-      <c r="Q34" s="160"/>
-      <c r="R34" s="160"/>
-      <c r="S34" s="160"/>
-      <c r="T34" s="160"/>
-      <c r="U34" s="160"/>
-      <c r="V34" s="160"/>
-      <c r="W34" s="160"/>
-    </row>
-    <row r="35" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="170"/>
+      <c r="L34" s="170"/>
+      <c r="M34" s="170"/>
+      <c r="N34" s="170"/>
+      <c r="O34" s="170"/>
+      <c r="P34" s="170"/>
+      <c r="Q34" s="170"/>
+      <c r="R34" s="170"/>
+      <c r="S34" s="170"/>
+      <c r="T34" s="170"/>
+      <c r="U34" s="170"/>
+      <c r="V34" s="170"/>
+      <c r="W34" s="170"/>
+    </row>
+    <row r="35" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20"/>
       <c r="B35" s="24"/>
       <c r="C35" s="23"/>
@@ -3514,7 +3508,7 @@
       <c r="V35" s="74"/>
       <c r="W35" s="74"/>
     </row>
-    <row r="36" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20"/>
       <c r="B36" s="24"/>
       <c r="C36" s="23"/>
@@ -3544,7 +3538,7 @@
       <c r="V36" s="74"/>
       <c r="W36" s="74"/>
     </row>
-    <row r="37" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="20"/>
       <c r="B37" s="24"/>
       <c r="C37" s="23"/>
@@ -3574,7 +3568,7 @@
       <c r="V37" s="74"/>
       <c r="W37" s="74"/>
     </row>
-    <row r="38" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="20"/>
       <c r="B38" s="24"/>
       <c r="C38" s="23"/>
@@ -3602,7 +3596,7 @@
       <c r="V38" s="74"/>
       <c r="W38" s="74"/>
     </row>
-    <row r="39" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="24"/>
       <c r="C39" s="23"/>
@@ -3630,7 +3624,7 @@
       <c r="V39" s="74"/>
       <c r="W39" s="74"/>
     </row>
-    <row r="40" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20"/>
       <c r="B40" s="24"/>
       <c r="C40" s="23"/>
@@ -3643,42 +3637,42 @@
       <c r="G40" s="94"/>
       <c r="H40" s="94"/>
       <c r="I40" s="74"/>
-      <c r="J40" s="168" t="s">
+      <c r="J40" s="208" t="s">
         <v>45</v>
       </c>
-      <c r="K40" s="157"/>
-      <c r="L40" s="158"/>
-      <c r="M40" s="180" t="str">
+      <c r="K40" s="133"/>
+      <c r="L40" s="149"/>
+      <c r="M40" s="157" t="str">
         <f>IF(SUM(J14:J33,M14:M33)=0,"",IF(M33&gt;0,N33,IF(M32&gt;0,N32,IF(M31&gt;0,N31,IF(M30&gt;0,N30,IF(M29&gt;0,N29,IF(M28&gt;0,N28,IF(M27&gt;0,N27,IF(M26&gt;0,N26,IF(M25&gt;0,N25,IF(M24&gt;0,N24,IF(M23&gt;0,N23,IF(M22&gt;0,N22,IF(M21&gt;0,N21,IF(M20&gt;0,N20,IF(M19&gt;0,N19,IF(M18&gt;0,N18,IF(M17&gt;0,N17,IF(M16&gt;0,N16,IF(M15&gt;0,N15,IF(M14&gt;0,N14,IF(J33&gt;0,K33,IF(J32&gt;0,K32,IF(J31&gt;0,K31,IF(J30&gt;0,K30,IF(J29&gt;0,K29,IF(J28&gt;0,K28,IF(J27&gt;0,K27,IF(J26&gt;0,K26,IF(J25&gt;0,K25,IF(J24&gt;0,K24,IF(J23&gt;0,K23,IF(J22&gt;0,K22,IF(J21&gt;0,K21,IF(J20&gt;0,K20,IF(J19&gt;0,K19,IF(J18&gt;0,K18,IF(J17&gt;0,K17,IF(J16&gt;0,K16,IF(J15&gt;0,K15,IF(J14&gt;0,K14)))))))))))))))))))))))))))))))))))))))))</f>
         <v/>
       </c>
-      <c r="N40" s="169" t="s">
+      <c r="N40" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="O40" s="194" t="str">
+      <c r="O40" s="174" t="str">
         <f>IF(SUM(L14:L33,O14:O33)=0,"",IF(O33&gt;0,N33,IF(O32&gt;0,N32,IF(O31&gt;0,N31,IF(O30&gt;0,N30,IF(O29&gt;0,N29,IF(O28&gt;0,N28,IF(O27&gt;0,N27,IF(O26&gt;0,N26,IF(O25&gt;0,N25,IF(O24&gt;0,N24,IF(O23&gt;0,N23,IF(O22&gt;0,N22,IF(O21&gt;0,N21,IF(O20&gt;0,N20,IF(O19&gt;0,N19,IF(O18&gt;0,N18,IF(O17&gt;0,N17,IF(O16&gt;0,N16,IF(O15&gt;0,N15,IF(O14&gt;0,N14,IF(L33&gt;0,K33,IF(L32&gt;0,K32,IF(L31&gt;0,K31,IF(L30&gt;0,K30,IF(L29&gt;0,K29,IF(L28&gt;0,K28,IF(L27&gt;0,K27,IF(L26&gt;0,K26,IF(L25&gt;0,K25,IF(L24&gt;0,K24,IF(L23&gt;0,K23,IF(L22&gt;0,K22,IF(L21&gt;0,K21,IF(L20&gt;0,K20,IF(L19&gt;0,K19,IF(L18&gt;0,K18,IF(L17&gt;0,K17,IF(L16&gt;0,K16,IF(L15&gt;0,K15,IF(L14&gt;0,K14)))))))))))))))))))))))))))))))))))))))))</f>
         <v/>
       </c>
-      <c r="P40" s="151"/>
-      <c r="Q40" s="191" t="s">
+      <c r="P40" s="198"/>
+      <c r="Q40" s="148" t="s">
         <v>46</v>
       </c>
-      <c r="R40" s="157"/>
-      <c r="S40" s="158"/>
-      <c r="T40" s="180" t="str">
+      <c r="R40" s="133"/>
+      <c r="S40" s="149"/>
+      <c r="T40" s="157" t="str">
         <f>IF(SUM(Q14:Q33,T14:T33)=0,"",IF(T33&gt;0,N33,IF(T32&gt;0,N32,IF(T31&gt;0,N31,IF(T30&gt;0,N30,IF(T29&gt;0,N29,IF(T28&gt;0,N28,IF(T27&gt;0,N27,IF(T26&gt;0,N26,IF(T25&gt;0,N25,IF(T24&gt;0,N24,IF(T23&gt;0,N23,IF(T22&gt;0,N22,IF(T21&gt;0,N21,IF(T20&gt;0,N20,IF(T19&gt;0,N19,IF(T18&gt;0,N18,IF(T17&gt;0,N17,IF(T16&gt;0,N16,IF(T15&gt;0,N15,IF(T14&gt;0,N14,IF(Q33&gt;0,K33,IF(Q32&gt;0,K32,IF(Q31&gt;0,K31,IF(Q30&gt;0,K30,IF(Q29&gt;0,K29,IF(Q28&gt;0,K28,IF(Q27&gt;0,K27,IF(Q26&gt;0,K26,IF(Q25&gt;0,K25,IF(Q24&gt;0,K24,IF(Q23&gt;0,K23,IF(Q22&gt;0,K22,IF(Q21&gt;0,K21,IF(Q20&gt;0,K20,IF(Q19&gt;0,K19,IF(Q18&gt;0,K18,IF(Q17&gt;0,K17,IF(Q16&gt;0,K16,IF(Q15&gt;0,K15,IF(Q14&gt;0,K14)))))))))))))))))))))))))))))))))))))))))</f>
         <v/>
       </c>
-      <c r="U40" s="169" t="s">
+      <c r="U40" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="V40" s="181" t="str">
+      <c r="V40" s="162" t="str">
         <f>IF(SUM(S14:S33,V14:V33)=0,"",IF(V33&gt;0,N33,IF(V32&gt;0,N32,IF(V31&gt;0,N31,IF(V30&gt;0,N30,IF(V29&gt;0,N29,IF(V28&gt;0,N28,IF(V27&gt;0,N27,IF(V26&gt;0,N26,IF(V25&gt;0,N25,IF(V24&gt;0,N24,IF(V23&gt;0,N23,IF(V22&gt;0,N22,IF(V21&gt;0,N21,IF(V20&gt;0,N20,IF(V19&gt;0,N19,IF(V18&gt;0,N18,IF(V17&gt;0,N17,IF(V16&gt;0,N16,IF(V15&gt;0,N15,IF(V14&gt;0,N14,IF(S33&gt;0,K33,IF(S32&gt;0,K32,IF(S31&gt;0,K31,IF(S30&gt;0,K30,IF(S29&gt;0,K29,IF(S28&gt;0,K28,IF(S27&gt;0,K27,IF(S26&gt;0,K26,IF(S25&gt;0,K25,IF(S24&gt;0,K24,IF(S23&gt;0,K23,IF(S22&gt;0,K22,IF(S21&gt;0,K21,IF(S20&gt;0,K20,IF(S19&gt;0,K19,IF(S18&gt;0,K18,IF(S17&gt;0,K17,IF(S16&gt;0,K16,IF(S15&gt;0,K15,IF(S14&gt;0,K14)))))))))))))))))))))))))))))))))))))))))</f>
         <v/>
       </c>
       <c r="W40" s="74"/>
     </row>
-    <row r="41" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="27"/>
       <c r="B41" s="25"/>
       <c r="C41" s="26"/>
@@ -3691,22 +3685,22 @@
       <c r="G41" s="95"/>
       <c r="H41" s="95"/>
       <c r="I41" s="74"/>
-      <c r="J41" s="162"/>
-      <c r="K41" s="163"/>
-      <c r="L41" s="164"/>
-      <c r="M41" s="173"/>
-      <c r="N41" s="163"/>
-      <c r="O41" s="164"/>
-      <c r="P41" s="152"/>
-      <c r="Q41" s="173"/>
-      <c r="R41" s="163"/>
-      <c r="S41" s="164"/>
-      <c r="T41" s="173"/>
-      <c r="U41" s="163"/>
-      <c r="V41" s="182"/>
+      <c r="J41" s="205"/>
+      <c r="K41" s="135"/>
+      <c r="L41" s="151"/>
+      <c r="M41" s="150"/>
+      <c r="N41" s="135"/>
+      <c r="O41" s="151"/>
+      <c r="P41" s="199"/>
+      <c r="Q41" s="150"/>
+      <c r="R41" s="135"/>
+      <c r="S41" s="151"/>
+      <c r="T41" s="150"/>
+      <c r="U41" s="135"/>
+      <c r="V41" s="163"/>
       <c r="W41" s="74"/>
     </row>
-    <row r="42" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="112" t="s">
         <v>34</v>
       </c>
@@ -3735,52 +3729,52 @@
         <v/>
       </c>
       <c r="I42" s="74"/>
-      <c r="J42" s="199" t="s">
+      <c r="J42" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="K42" s="196"/>
-      <c r="L42" s="200"/>
-      <c r="M42" s="188" t="str">
+      <c r="K42" s="137"/>
+      <c r="L42" s="138"/>
+      <c r="M42" s="152" t="str">
         <f>IF(M40="","",IF(M40&gt;O40,1,0))</f>
         <v/>
       </c>
-      <c r="N42" s="204" t="s">
+      <c r="N42" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="O42" s="207" t="str">
+      <c r="O42" s="153" t="str">
         <f>IF(O40="","",IF(O40&gt;M40,1,0))</f>
         <v/>
       </c>
-      <c r="P42" s="152"/>
-      <c r="Q42" s="205" t="s">
+      <c r="P42" s="199"/>
+      <c r="Q42" s="143" t="s">
         <v>47</v>
       </c>
-      <c r="R42" s="196"/>
-      <c r="S42" s="200"/>
-      <c r="T42" s="188" t="str">
+      <c r="R42" s="137"/>
+      <c r="S42" s="138"/>
+      <c r="T42" s="152" t="str">
         <f>IF(T40="","",IF(T40&gt;V40,1,0))</f>
         <v/>
       </c>
-      <c r="U42" s="204" t="s">
+      <c r="U42" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="V42" s="189" t="str">
+      <c r="V42" s="168" t="str">
         <f>IF(V40="","",IF(V40&gt;T40,1,0))</f>
         <v/>
       </c>
       <c r="W42" s="74"/>
     </row>
-    <row r="43" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="115" t="s">
         <v>35</v>
       </c>
       <c r="B43" s="116"/>
       <c r="C43" s="117"/>
-      <c r="D43" s="145" t="s">
+      <c r="D43" s="192" t="s">
         <v>37</v>
       </c>
-      <c r="E43" s="146"/>
-      <c r="F43" s="147"/>
+      <c r="E43" s="193"/>
+      <c r="F43" s="194"/>
       <c r="G43" s="118" t="s">
         <v>38</v>
       </c>
@@ -3788,61 +3782,61 @@
         <v>39</v>
       </c>
       <c r="I43" s="74"/>
-      <c r="J43" s="201"/>
-      <c r="K43" s="202"/>
-      <c r="L43" s="203"/>
-      <c r="M43" s="185"/>
-      <c r="N43" s="202"/>
-      <c r="O43" s="203"/>
-      <c r="P43" s="153"/>
-      <c r="Q43" s="185"/>
-      <c r="R43" s="202"/>
-      <c r="S43" s="203"/>
-      <c r="T43" s="185"/>
-      <c r="U43" s="202"/>
-      <c r="V43" s="187"/>
+      <c r="J43" s="139"/>
+      <c r="K43" s="140"/>
+      <c r="L43" s="141"/>
+      <c r="M43" s="144"/>
+      <c r="N43" s="140"/>
+      <c r="O43" s="141"/>
+      <c r="P43" s="200"/>
+      <c r="Q43" s="144"/>
+      <c r="R43" s="140"/>
+      <c r="S43" s="141"/>
+      <c r="T43" s="144"/>
+      <c r="U43" s="140"/>
+      <c r="V43" s="167"/>
       <c r="W43" s="74"/>
     </row>
-    <row r="44" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="206" t="s">
+    <row r="44" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="145" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="133"/>
-      <c r="C44" s="134"/>
-      <c r="D44" s="148"/>
-      <c r="E44" s="149"/>
-      <c r="F44" s="150"/>
+      <c r="B44" s="146"/>
+      <c r="C44" s="147"/>
+      <c r="D44" s="195"/>
+      <c r="E44" s="196"/>
+      <c r="F44" s="197"/>
       <c r="G44" s="94"/>
       <c r="H44" s="94"/>
       <c r="I44" s="74"/>
-      <c r="J44" s="156" t="s">
+      <c r="J44" s="203" t="s">
         <v>48</v>
       </c>
-      <c r="K44" s="157"/>
-      <c r="L44" s="157"/>
-      <c r="M44" s="157"/>
-      <c r="N44" s="157"/>
-      <c r="O44" s="157"/>
-      <c r="P44" s="158"/>
-      <c r="Q44" s="191" t="s">
+      <c r="K44" s="133"/>
+      <c r="L44" s="133"/>
+      <c r="M44" s="133"/>
+      <c r="N44" s="133"/>
+      <c r="O44" s="133"/>
+      <c r="P44" s="149"/>
+      <c r="Q44" s="148" t="s">
         <v>49</v>
       </c>
-      <c r="R44" s="157"/>
-      <c r="S44" s="158"/>
-      <c r="T44" s="180" t="str">
+      <c r="R44" s="133"/>
+      <c r="S44" s="149"/>
+      <c r="T44" s="157" t="str">
         <f>IF(AND(K48="",L48="",M48="",N48="",O48="",K50="",L50="",M50="",N50="",O50=""),"",SUM(K50:V50))</f>
         <v/>
       </c>
-      <c r="U44" s="169" t="s">
+      <c r="U44" s="155" t="s">
         <v>19</v>
       </c>
-      <c r="V44" s="181" t="str">
+      <c r="V44" s="162" t="str">
         <f>IF(AND(K52="",L52="",M52="",N52="",O52="",K54="",L54="",M54="",N54="",O54=""),"",SUM(K54:V54))</f>
         <v/>
       </c>
       <c r="W44" s="74"/>
     </row>
-    <row r="45" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="36"/>
       <c r="B45" s="46"/>
       <c r="C45" s="46"/>
@@ -3852,23 +3846,23 @@
       <c r="G45" s="74"/>
       <c r="H45" s="74"/>
       <c r="I45" s="74"/>
-      <c r="J45" s="159"/>
-      <c r="K45" s="160"/>
-      <c r="L45" s="160"/>
-      <c r="M45" s="160"/>
-      <c r="N45" s="160"/>
-      <c r="O45" s="160"/>
-      <c r="P45" s="161"/>
-      <c r="Q45" s="173"/>
-      <c r="R45" s="163"/>
-      <c r="S45" s="164"/>
-      <c r="T45" s="210"/>
-      <c r="U45" s="209"/>
-      <c r="V45" s="183"/>
+      <c r="J45" s="204"/>
+      <c r="K45" s="170"/>
+      <c r="L45" s="170"/>
+      <c r="M45" s="170"/>
+      <c r="N45" s="170"/>
+      <c r="O45" s="170"/>
+      <c r="P45" s="177"/>
+      <c r="Q45" s="150"/>
+      <c r="R45" s="135"/>
+      <c r="S45" s="151"/>
+      <c r="T45" s="158"/>
+      <c r="U45" s="156"/>
+      <c r="V45" s="164"/>
       <c r="W45" s="74"/>
       <c r="X45" s="4"/>
     </row>
-    <row r="46" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="36"/>
       <c r="B46" s="74"/>
       <c r="C46" s="74"/>
@@ -3878,78 +3872,78 @@
       <c r="G46" s="74"/>
       <c r="H46" s="74"/>
       <c r="I46" s="74"/>
-      <c r="J46" s="162"/>
-      <c r="K46" s="163"/>
-      <c r="L46" s="163"/>
-      <c r="M46" s="163"/>
-      <c r="N46" s="163"/>
-      <c r="O46" s="163"/>
-      <c r="P46" s="164"/>
-      <c r="Q46" s="195" t="s">
+      <c r="J46" s="205"/>
+      <c r="K46" s="135"/>
+      <c r="L46" s="135"/>
+      <c r="M46" s="135"/>
+      <c r="N46" s="135"/>
+      <c r="O46" s="135"/>
+      <c r="P46" s="151"/>
+      <c r="Q46" s="175" t="s">
         <v>47</v>
       </c>
-      <c r="R46" s="196"/>
-      <c r="S46" s="196"/>
-      <c r="T46" s="184" t="str">
+      <c r="R46" s="137"/>
+      <c r="S46" s="137"/>
+      <c r="T46" s="165" t="str">
         <f>IF(T44="","",IF(T44&gt;V44,1,0))</f>
         <v/>
       </c>
-      <c r="U46" s="208" t="s">
+      <c r="U46" s="154" t="s">
         <v>19</v>
       </c>
-      <c r="V46" s="186" t="str">
+      <c r="V46" s="166" t="str">
         <f>IF(V44="","",IF(T44&lt;X44,1,0))</f>
         <v/>
       </c>
       <c r="W46" s="74"/>
     </row>
-    <row r="47" spans="1:24" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="36"/>
       <c r="B47" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="198" t="s">
+      <c r="C47" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="163"/>
-      <c r="E47" s="198" t="s">
+      <c r="D47" s="135"/>
+      <c r="E47" s="134" t="s">
         <v>52</v>
       </c>
-      <c r="F47" s="163"/>
-      <c r="G47" s="163"/>
-      <c r="H47" s="163"/>
+      <c r="F47" s="135"/>
+      <c r="G47" s="135"/>
+      <c r="H47" s="135"/>
       <c r="I47" s="74"/>
-      <c r="J47" s="138" t="s">
+      <c r="J47" s="188" t="s">
         <v>53</v>
       </c>
-      <c r="K47" s="139"/>
-      <c r="L47" s="192" t="str">
+      <c r="K47" s="172"/>
+      <c r="L47" s="171" t="str">
         <f>IF(B8="","",B8)</f>
         <v/>
       </c>
-      <c r="M47" s="139"/>
-      <c r="N47" s="139"/>
-      <c r="O47" s="139"/>
-      <c r="P47" s="193"/>
-      <c r="Q47" s="173"/>
-      <c r="R47" s="163"/>
-      <c r="S47" s="163"/>
-      <c r="T47" s="185"/>
-      <c r="U47" s="202"/>
-      <c r="V47" s="187"/>
+      <c r="M47" s="172"/>
+      <c r="N47" s="172"/>
+      <c r="O47" s="172"/>
+      <c r="P47" s="173"/>
+      <c r="Q47" s="150"/>
+      <c r="R47" s="135"/>
+      <c r="S47" s="135"/>
+      <c r="T47" s="144"/>
+      <c r="U47" s="140"/>
+      <c r="V47" s="167"/>
       <c r="W47" s="74"/>
     </row>
-    <row r="48" spans="1:24" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="50">
         <v>1</v>
       </c>
       <c r="B48" s="106"/>
       <c r="C48" s="106"/>
       <c r="D48" s="107"/>
-      <c r="E48" s="132"/>
-      <c r="F48" s="133"/>
-      <c r="G48" s="133"/>
-      <c r="H48" s="134"/>
+      <c r="E48" s="209"/>
+      <c r="F48" s="146"/>
+      <c r="G48" s="146"/>
+      <c r="H48" s="147"/>
       <c r="I48" s="74"/>
       <c r="J48" s="30" t="s">
         <v>26</v>
@@ -3968,17 +3962,17 @@
       <c r="V48" s="99"/>
       <c r="W48" s="74"/>
     </row>
-    <row r="49" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="50">
         <v>2</v>
       </c>
       <c r="B49" s="108"/>
       <c r="C49" s="106"/>
       <c r="D49" s="107"/>
-      <c r="E49" s="132"/>
-      <c r="F49" s="133"/>
-      <c r="G49" s="133"/>
-      <c r="H49" s="134"/>
+      <c r="E49" s="209"/>
+      <c r="F49" s="146"/>
+      <c r="G49" s="146"/>
+      <c r="H49" s="147"/>
       <c r="I49" s="74"/>
       <c r="J49" s="29" t="s">
         <v>54</v>
@@ -3997,17 +3991,17 @@
       <c r="V49" s="101"/>
       <c r="W49" s="74"/>
     </row>
-    <row r="50" spans="1:23" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="36"/>
       <c r="B50" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="135"/>
-      <c r="D50" s="133"/>
-      <c r="E50" s="133"/>
-      <c r="F50" s="133"/>
-      <c r="G50" s="133"/>
-      <c r="H50" s="133"/>
+      <c r="C50" s="210"/>
+      <c r="D50" s="146"/>
+      <c r="E50" s="146"/>
+      <c r="F50" s="146"/>
+      <c r="G50" s="146"/>
+      <c r="H50" s="146"/>
       <c r="I50" s="74"/>
       <c r="J50" s="31" t="s">
         <v>28</v>
@@ -4026,30 +4020,30 @@
       <c r="V50" s="103"/>
       <c r="W50" s="74"/>
     </row>
-    <row r="51" spans="1:23" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" ht="16.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="50">
         <v>1</v>
       </c>
       <c r="B51" s="106"/>
       <c r="C51" s="106"/>
       <c r="D51" s="107"/>
-      <c r="E51" s="132"/>
-      <c r="F51" s="133"/>
-      <c r="G51" s="133"/>
-      <c r="H51" s="134"/>
+      <c r="E51" s="209"/>
+      <c r="F51" s="146"/>
+      <c r="G51" s="146"/>
+      <c r="H51" s="147"/>
       <c r="I51" s="74"/>
-      <c r="J51" s="140" t="s">
+      <c r="J51" s="189" t="s">
         <v>56</v>
       </c>
-      <c r="K51" s="137"/>
-      <c r="L51" s="136" t="str">
+      <c r="K51" s="160"/>
+      <c r="L51" s="187" t="str">
         <f>IF(G8="","",G8)</f>
         <v/>
       </c>
-      <c r="M51" s="137"/>
-      <c r="N51" s="137"/>
-      <c r="O51" s="137"/>
-      <c r="P51" s="137"/>
+      <c r="M51" s="160"/>
+      <c r="N51" s="160"/>
+      <c r="O51" s="160"/>
+      <c r="P51" s="160"/>
       <c r="Q51" s="28"/>
       <c r="R51" s="28"/>
       <c r="S51" s="28"/>
@@ -4058,17 +4052,17 @@
       <c r="V51" s="32"/>
       <c r="W51" s="74"/>
     </row>
-    <row r="52" spans="1:23" ht="16.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="50">
         <v>2</v>
       </c>
       <c r="B52" s="108"/>
       <c r="C52" s="108"/>
       <c r="D52" s="110"/>
-      <c r="E52" s="132"/>
-      <c r="F52" s="133"/>
-      <c r="G52" s="133"/>
-      <c r="H52" s="134"/>
+      <c r="E52" s="209"/>
+      <c r="F52" s="146"/>
+      <c r="G52" s="146"/>
+      <c r="H52" s="147"/>
       <c r="I52" s="74"/>
       <c r="J52" s="30" t="s">
         <v>26</v>
@@ -4087,7 +4081,7 @@
       <c r="V52" s="98"/>
       <c r="W52" s="74"/>
     </row>
-    <row r="53" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="36"/>
       <c r="B53" s="109" t="s">
         <v>57</v>
@@ -4116,15 +4110,15 @@
       <c r="V53" s="101"/>
       <c r="W53" s="74"/>
     </row>
-    <row r="54" spans="1:23" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="36"/>
       <c r="B54" s="106"/>
       <c r="C54" s="106"/>
       <c r="D54" s="107"/>
-      <c r="E54" s="132"/>
-      <c r="F54" s="133"/>
-      <c r="G54" s="133"/>
-      <c r="H54" s="134"/>
+      <c r="E54" s="209"/>
+      <c r="F54" s="146"/>
+      <c r="G54" s="146"/>
+      <c r="H54" s="147"/>
       <c r="I54" s="74"/>
       <c r="J54" s="31" t="s">
         <v>28</v>
@@ -4143,7 +4137,7 @@
       <c r="V54" s="103"/>
       <c r="W54" s="74"/>
     </row>
-    <row r="55" spans="1:23" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" s="3" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="52"/>
       <c r="B55" s="53"/>
       <c r="C55" s="53"/>
@@ -4153,24 +4147,24 @@
       <c r="G55" s="53"/>
       <c r="H55" s="53"/>
       <c r="I55" s="53"/>
-      <c r="J55" s="197" t="s">
+      <c r="J55" s="132" t="s">
         <v>58</v>
       </c>
-      <c r="K55" s="157"/>
-      <c r="L55" s="157"/>
-      <c r="M55" s="157"/>
-      <c r="N55" s="157"/>
-      <c r="O55" s="157"/>
-      <c r="P55" s="157"/>
-      <c r="Q55" s="157"/>
-      <c r="R55" s="157"/>
-      <c r="S55" s="157"/>
-      <c r="T55" s="157"/>
-      <c r="U55" s="157"/>
-      <c r="V55" s="157"/>
+      <c r="K55" s="133"/>
+      <c r="L55" s="133"/>
+      <c r="M55" s="133"/>
+      <c r="N55" s="133"/>
+      <c r="O55" s="133"/>
+      <c r="P55" s="133"/>
+      <c r="Q55" s="133"/>
+      <c r="R55" s="133"/>
+      <c r="S55" s="133"/>
+      <c r="T55" s="133"/>
+      <c r="U55" s="133"/>
+      <c r="V55" s="133"/>
       <c r="W55" s="53"/>
     </row>
-    <row r="56" spans="1:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="36"/>
       <c r="B56" s="39" t="s">
         <v>59</v>
@@ -4219,7 +4213,7 @@
       </c>
       <c r="W56" s="74"/>
     </row>
-    <row r="57" spans="1:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="36"/>
       <c r="B57" s="40"/>
       <c r="C57" s="55" t="s">
@@ -4262,7 +4256,7 @@
       </c>
       <c r="W57" s="74"/>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="36"/>
       <c r="B58" s="74"/>
       <c r="C58" s="74"/>
@@ -4289,7 +4283,7 @@
       </c>
       <c r="W58" s="74"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" s="36"/>
       <c r="B59" s="74"/>
       <c r="C59" s="74"/>
@@ -4314,7 +4308,7 @@
       <c r="V59" s="74"/>
       <c r="W59" s="74"/>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="36"/>
       <c r="B60" s="74"/>
       <c r="C60" s="74"/>
@@ -4341,20 +4335,36 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="J55:V55"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="J42:L43"/>
-    <mergeCell ref="N42:N43"/>
-    <mergeCell ref="Q42:S43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="Q44:S45"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="O42:O43"/>
-    <mergeCell ref="U46:U47"/>
-    <mergeCell ref="U42:U43"/>
-    <mergeCell ref="U44:U45"/>
-    <mergeCell ref="T44:T45"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="E49:H49"/>
+    <mergeCell ref="E51:H51"/>
+    <mergeCell ref="E52:H52"/>
+    <mergeCell ref="E54:H54"/>
+    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="D26:F27"/>
+    <mergeCell ref="D43:F44"/>
+    <mergeCell ref="P40:P43"/>
+    <mergeCell ref="N9:P9"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="J44:P46"/>
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="J40:L41"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="T8:T10"/>
+    <mergeCell ref="U8:U10"/>
+    <mergeCell ref="V8:V10"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="G8:P8"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="G7:P7"/>
     <mergeCell ref="Q12:V12"/>
     <mergeCell ref="T40:T41"/>
     <mergeCell ref="V40:V41"/>
@@ -4370,39 +4380,23 @@
     <mergeCell ref="L47:P47"/>
     <mergeCell ref="O40:O41"/>
     <mergeCell ref="Q46:S47"/>
-    <mergeCell ref="B3:E5"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="G8:P8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="T8:T10"/>
-    <mergeCell ref="U8:U10"/>
-    <mergeCell ref="V8:V10"/>
-    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J55:V55"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="J42:L43"/>
+    <mergeCell ref="N42:N43"/>
+    <mergeCell ref="Q42:S43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="Q44:S45"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="O42:O43"/>
+    <mergeCell ref="U46:U47"/>
+    <mergeCell ref="U42:U43"/>
+    <mergeCell ref="U44:U45"/>
+    <mergeCell ref="T44:T45"/>
     <mergeCell ref="L51:P51"/>
-    <mergeCell ref="J47:K47"/>
     <mergeCell ref="J51:K51"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="G7:P7"/>
-    <mergeCell ref="D26:F27"/>
-    <mergeCell ref="D43:F44"/>
-    <mergeCell ref="P40:P43"/>
-    <mergeCell ref="N9:P9"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="J44:P46"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="J40:L41"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="E49:H49"/>
-    <mergeCell ref="E51:H51"/>
-    <mergeCell ref="E52:H52"/>
-    <mergeCell ref="E54:H54"/>
-    <mergeCell ref="C50:H50"/>
   </mergeCells>
   <conditionalFormatting sqref="E13:H24">
     <cfRule type="containsText" dxfId="11" priority="19" operator="containsText" text="X">

</xml_diff>